<commit_message>
Update Master File of 1 sec to 10 min
Update 1 sec to 10 min master file
</commit_message>
<xml_diff>
--- a/src/test/DataFiles/ConvertedFileVarsha.xlsx
+++ b/src/test/DataFiles/ConvertedFileVarsha.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="297">
   <si>
     <t>1294.7074</t>
   </si>
@@ -91,6 +91,837 @@
   </si>
   <si>
     <t>39.986004</t>
+  </si>
+  <si>
+    <t>2551.1846</t>
+  </si>
+  <si>
+    <t>2551.8374</t>
+  </si>
+  <si>
+    <t>2551.8958</t>
+  </si>
+  <si>
+    <t>2551.904</t>
+  </si>
+  <si>
+    <t>2551.8948</t>
+  </si>
+  <si>
+    <t>2551.923</t>
+  </si>
+  <si>
+    <t>2551.9004</t>
+  </si>
+  <si>
+    <t>2552.0522</t>
+  </si>
+  <si>
+    <t>2551.9158</t>
+  </si>
+  <si>
+    <t>2551.905</t>
+  </si>
+  <si>
+    <t>2551.9639</t>
+  </si>
+  <si>
+    <t>2551.8577</t>
+  </si>
+  <si>
+    <t>2551.8843</t>
+  </si>
+  <si>
+    <t>2551.859</t>
+  </si>
+  <si>
+    <t>2552.0032</t>
+  </si>
+  <si>
+    <t>1275.0472</t>
+  </si>
+  <si>
+    <t>1678.0795</t>
+  </si>
+  <si>
+    <t>2090.0742</t>
+  </si>
+  <si>
+    <t>2176.9404</t>
+  </si>
+  <si>
+    <t>2368.494</t>
+  </si>
+  <si>
+    <t>2492.396</t>
+  </si>
+  <si>
+    <t>2547.9219</t>
+  </si>
+  <si>
+    <t>2551.9636</t>
+  </si>
+  <si>
+    <t>2551.8752</t>
+  </si>
+  <si>
+    <t>2551.8875</t>
+  </si>
+  <si>
+    <t>2551.8616</t>
+  </si>
+  <si>
+    <t>2551.9978</t>
+  </si>
+  <si>
+    <t>2543.6296</t>
+  </si>
+  <si>
+    <t>2408.5933</t>
+  </si>
+  <si>
+    <t>2423.2705</t>
+  </si>
+  <si>
+    <t>2246.3098</t>
+  </si>
+  <si>
+    <t>2003.5913</t>
+  </si>
+  <si>
+    <t>2366.4531</t>
+  </si>
+  <si>
+    <t>22.285994</t>
+  </si>
+  <si>
+    <t>22.358547</t>
+  </si>
+  <si>
+    <t>22.538628</t>
+  </si>
+  <si>
+    <t>22.537216</t>
+  </si>
+  <si>
+    <t>22.695967</t>
+  </si>
+  <si>
+    <t>22.68591</t>
+  </si>
+  <si>
+    <t>22.812077</t>
+  </si>
+  <si>
+    <t>23.002375</t>
+  </si>
+  <si>
+    <t>23.117111</t>
+  </si>
+  <si>
+    <t>23.115757</t>
+  </si>
+  <si>
+    <t>23.121675</t>
+  </si>
+  <si>
+    <t>22.974781</t>
+  </si>
+  <si>
+    <t>22.845783</t>
+  </si>
+  <si>
+    <t>22.858955</t>
+  </si>
+  <si>
+    <t>22.90194</t>
+  </si>
+  <si>
+    <t>23.121311</t>
+  </si>
+  <si>
+    <t>23.098015</t>
+  </si>
+  <si>
+    <t>23.099894</t>
+  </si>
+  <si>
+    <t>23.159678</t>
+  </si>
+  <si>
+    <t>23.204374</t>
+  </si>
+  <si>
+    <t>23.267136</t>
+  </si>
+  <si>
+    <t>23.367588</t>
+  </si>
+  <si>
+    <t>23.412777</t>
+  </si>
+  <si>
+    <t>23.382523</t>
+  </si>
+  <si>
+    <t>23.310095</t>
+  </si>
+  <si>
+    <t>23.26742</t>
+  </si>
+  <si>
+    <t>23.14317</t>
+  </si>
+  <si>
+    <t>22.972858</t>
+  </si>
+  <si>
+    <t>22.832315</t>
+  </si>
+  <si>
+    <t>22.712816</t>
+  </si>
+  <si>
+    <t>22.590076</t>
+  </si>
+  <si>
+    <t>22.405539</t>
+  </si>
+  <si>
+    <t>22.342806</t>
+  </si>
+  <si>
+    <t>10.203386</t>
+  </si>
+  <si>
+    <t>10.421573</t>
+  </si>
+  <si>
+    <t>10.858782</t>
+  </si>
+  <si>
+    <t>10.681835</t>
+  </si>
+  <si>
+    <t>10.972407</t>
+  </si>
+  <si>
+    <t>10.746028</t>
+  </si>
+  <si>
+    <t>10.963142</t>
+  </si>
+  <si>
+    <t>11.371295</t>
+  </si>
+  <si>
+    <t>11.25637</t>
+  </si>
+  <si>
+    <t>11.235619</t>
+  </si>
+  <si>
+    <t>11.279897</t>
+  </si>
+  <si>
+    <t>10.832786</t>
+  </si>
+  <si>
+    <t>10.747735</t>
+  </si>
+  <si>
+    <t>11.012778</t>
+  </si>
+  <si>
+    <t>11.278642</t>
+  </si>
+  <si>
+    <t>7.712447</t>
+  </si>
+  <si>
+    <t>8.338399</t>
+  </si>
+  <si>
+    <t>9.060881</t>
+  </si>
+  <si>
+    <t>9.120451</t>
+  </si>
+  <si>
+    <t>9.586052</t>
+  </si>
+  <si>
+    <t>9.765484</t>
+  </si>
+  <si>
+    <t>9.933974</t>
+  </si>
+  <si>
+    <t>9.901523</t>
+  </si>
+  <si>
+    <t>10.153263</t>
+  </si>
+  <si>
+    <t>10.16539</t>
+  </si>
+  <si>
+    <t>10.247307</t>
+  </si>
+  <si>
+    <t>10.197335</t>
+  </si>
+  <si>
+    <t>9.791318</t>
+  </si>
+  <si>
+    <t>9.494891</t>
+  </si>
+  <si>
+    <t>9.408595</t>
+  </si>
+  <si>
+    <t>9.11242</t>
+  </si>
+  <si>
+    <t>8.7769785</t>
+  </si>
+  <si>
+    <t>9.471659</t>
+  </si>
+  <si>
+    <t>26.800062</t>
+  </si>
+  <si>
+    <t>35.172127</t>
+  </si>
+  <si>
+    <t>38.452316</t>
+  </si>
+  <si>
+    <t>29.230577</t>
+  </si>
+  <si>
+    <t>30.400446</t>
+  </si>
+  <si>
+    <t>37.093224</t>
+  </si>
+  <si>
+    <t>32.047356</t>
+  </si>
+  <si>
+    <t>39.62617</t>
+  </si>
+  <si>
+    <t>33.247257</t>
+  </si>
+  <si>
+    <t>36.150204</t>
+  </si>
+  <si>
+    <t>35.465755</t>
+  </si>
+  <si>
+    <t>36.578808</t>
+  </si>
+  <si>
+    <t>32.187283</t>
+  </si>
+  <si>
+    <t>35.6066</t>
+  </si>
+  <si>
+    <t>37.584923</t>
+  </si>
+  <si>
+    <t>45.86213</t>
+  </si>
+  <si>
+    <t>27.42082</t>
+  </si>
+  <si>
+    <t>25.873362</t>
+  </si>
+  <si>
+    <t>27.887178</t>
+  </si>
+  <si>
+    <t>36.165817</t>
+  </si>
+  <si>
+    <t>27.088913</t>
+  </si>
+  <si>
+    <t>39.324482</t>
+  </si>
+  <si>
+    <t>43.104813</t>
+  </si>
+  <si>
+    <t>40.043167</t>
+  </si>
+  <si>
+    <t>42.98627</t>
+  </si>
+  <si>
+    <t>31.499195</t>
+  </si>
+  <si>
+    <t>29.077686</t>
+  </si>
+  <si>
+    <t>29.725286</t>
+  </si>
+  <si>
+    <t>37.543438</t>
+  </si>
+  <si>
+    <t>29.468283</t>
+  </si>
+  <si>
+    <t>31.059917</t>
+  </si>
+  <si>
+    <t>37.67543</t>
+  </si>
+  <si>
+    <t>38.303127</t>
+  </si>
+  <si>
+    <t>2367.0867</t>
+  </si>
+  <si>
+    <t>2551.1853</t>
+  </si>
+  <si>
+    <t>2551.84</t>
+  </si>
+  <si>
+    <t>2551.8936</t>
+  </si>
+  <si>
+    <t>2551.9055</t>
+  </si>
+  <si>
+    <t>2551.8965</t>
+  </si>
+  <si>
+    <t>2551.9192</t>
+  </si>
+  <si>
+    <t>2552.0513</t>
+  </si>
+  <si>
+    <t>2551.914</t>
+  </si>
+  <si>
+    <t>2551.909</t>
+  </si>
+  <si>
+    <t>2551.9624</t>
+  </si>
+  <si>
+    <t>2551.8574</t>
+  </si>
+  <si>
+    <t>2551.8833</t>
+  </si>
+  <si>
+    <t>2551.858</t>
+  </si>
+  <si>
+    <t>2552.0044</t>
+  </si>
+  <si>
+    <t>1294.9879</t>
+  </si>
+  <si>
+    <t>1496.2748</t>
+  </si>
+  <si>
+    <t>1451.9669</t>
+  </si>
+  <si>
+    <t>1182.9359</t>
+  </si>
+  <si>
+    <t>1275.9205</t>
+  </si>
+  <si>
+    <t>1679.0857</t>
+  </si>
+  <si>
+    <t>2089.9944</t>
+  </si>
+  <si>
+    <t>2177.1272</t>
+  </si>
+  <si>
+    <t>2368.873</t>
+  </si>
+  <si>
+    <t>2492.656</t>
+  </si>
+  <si>
+    <t>2547.923</t>
+  </si>
+  <si>
+    <t>2551.9617</t>
+  </si>
+  <si>
+    <t>2551.8743</t>
+  </si>
+  <si>
+    <t>2551.8894</t>
+  </si>
+  <si>
+    <t>2551.8623</t>
+  </si>
+  <si>
+    <t>2551.9956</t>
+  </si>
+  <si>
+    <t>2543.445</t>
+  </si>
+  <si>
+    <t>2408.6497</t>
+  </si>
+  <si>
+    <t>2423.2156</t>
+  </si>
+  <si>
+    <t>2245.9329</t>
+  </si>
+  <si>
+    <t>2003.5146</t>
+  </si>
+  <si>
+    <t>22.342758</t>
+  </si>
+  <si>
+    <t>22.286045</t>
+  </si>
+  <si>
+    <t>22.35879</t>
+  </si>
+  <si>
+    <t>22.538855</t>
+  </si>
+  <si>
+    <t>22.537374</t>
+  </si>
+  <si>
+    <t>22.695833</t>
+  </si>
+  <si>
+    <t>22.686129</t>
+  </si>
+  <si>
+    <t>22.81207</t>
+  </si>
+  <si>
+    <t>23.00305</t>
+  </si>
+  <si>
+    <t>23.11686</t>
+  </si>
+  <si>
+    <t>23.116068</t>
+  </si>
+  <si>
+    <t>23.12152</t>
+  </si>
+  <si>
+    <t>22.97449</t>
+  </si>
+  <si>
+    <t>22.845627</t>
+  </si>
+  <si>
+    <t>22.859112</t>
+  </si>
+  <si>
+    <t>22.901943</t>
+  </si>
+  <si>
+    <t>23.95853</t>
+  </si>
+  <si>
+    <t>23.719341</t>
+  </si>
+  <si>
+    <t>23.481483</t>
+  </si>
+  <si>
+    <t>23.316998</t>
+  </si>
+  <si>
+    <t>23.121143</t>
+  </si>
+  <si>
+    <t>23.15984</t>
+  </si>
+  <si>
+    <t>23.20438</t>
+  </si>
+  <si>
+    <t>23.267328</t>
+  </si>
+  <si>
+    <t>23.367725</t>
+  </si>
+  <si>
+    <t>23.412783</t>
+  </si>
+  <si>
+    <t>23.382364</t>
+  </si>
+  <si>
+    <t>23.310074</t>
+  </si>
+  <si>
+    <t>23.267307</t>
+  </si>
+  <si>
+    <t>23.14296</t>
+  </si>
+  <si>
+    <t>22.97257</t>
+  </si>
+  <si>
+    <t>22.831934</t>
+  </si>
+  <si>
+    <t>22.71281</t>
+  </si>
+  <si>
+    <t>22.58973</t>
+  </si>
+  <si>
+    <t>22.405218</t>
+  </si>
+  <si>
+    <t>9.473169</t>
+  </si>
+  <si>
+    <t>10.201378</t>
+  </si>
+  <si>
+    <t>10.420978</t>
+  </si>
+  <si>
+    <t>10.860309</t>
+  </si>
+  <si>
+    <t>10.681615</t>
+  </si>
+  <si>
+    <t>10.973873</t>
+  </si>
+  <si>
+    <t>10.743506</t>
+  </si>
+  <si>
+    <t>10.964289</t>
+  </si>
+  <si>
+    <t>11.373878</t>
+  </si>
+  <si>
+    <t>11.255144</t>
+  </si>
+  <si>
+    <t>11.236181</t>
+  </si>
+  <si>
+    <t>11.279349</t>
+  </si>
+  <si>
+    <t>10.831766</t>
+  </si>
+  <si>
+    <t>10.7473545</t>
+  </si>
+  <si>
+    <t>11.012513</t>
+  </si>
+  <si>
+    <t>11.280294</t>
+  </si>
+  <si>
+    <t>7.720681</t>
+  </si>
+  <si>
+    <t>8.208365</t>
+  </si>
+  <si>
+    <t>8.0372095</t>
+  </si>
+  <si>
+    <t>7.5369325</t>
+  </si>
+  <si>
+    <t>7.7136006</t>
+  </si>
+  <si>
+    <t>8.339524</t>
+  </si>
+  <si>
+    <t>9.060338</t>
+  </si>
+  <si>
+    <t>9.121701</t>
+  </si>
+  <si>
+    <t>9.58663</t>
+  </si>
+  <si>
+    <t>9.765351</t>
+  </si>
+  <si>
+    <t>9.935642</t>
+  </si>
+  <si>
+    <t>9.902531</t>
+  </si>
+  <si>
+    <t>10.151157</t>
+  </si>
+  <si>
+    <t>10.166868</t>
+  </si>
+  <si>
+    <t>10.248204</t>
+  </si>
+  <si>
+    <t>10.194911</t>
+  </si>
+  <si>
+    <t>9.790235</t>
+  </si>
+  <si>
+    <t>9.495918</t>
+  </si>
+  <si>
+    <t>9.40916</t>
+  </si>
+  <si>
+    <t>9.110135</t>
+  </si>
+  <si>
+    <t>8.779959</t>
+  </si>
+  <si>
+    <t>38.31041</t>
+  </si>
+  <si>
+    <t>26.804865</t>
+  </si>
+  <si>
+    <t>35.15529</t>
+  </si>
+  <si>
+    <t>38.4976</t>
+  </si>
+  <si>
+    <t>29.202595</t>
+  </si>
+  <si>
+    <t>30.40269</t>
+  </si>
+  <si>
+    <t>37.08652</t>
+  </si>
+  <si>
+    <t>32.055054</t>
+  </si>
+  <si>
+    <t>39.642864</t>
+  </si>
+  <si>
+    <t>33.233765</t>
+  </si>
+  <si>
+    <t>36.146774</t>
+  </si>
+  <si>
+    <t>35.483994</t>
+  </si>
+  <si>
+    <t>36.554363</t>
+  </si>
+  <si>
+    <t>32.1983</t>
+  </si>
+  <si>
+    <t>35.6069</t>
+  </si>
+  <si>
+    <t>37.603806</t>
+  </si>
+  <si>
+    <t>111.21471</t>
+  </si>
+  <si>
+    <t>86.801865</t>
+  </si>
+  <si>
+    <t>118.2626</t>
+  </si>
+  <si>
+    <t>99.66519</t>
+  </si>
+  <si>
+    <t>45.870255</t>
+  </si>
+  <si>
+    <t>27.419693</t>
+  </si>
+  <si>
+    <t>25.881853</t>
+  </si>
+  <si>
+    <t>27.896704</t>
+  </si>
+  <si>
+    <t>36.161747</t>
+  </si>
+  <si>
+    <t>27.066954</t>
+  </si>
+  <si>
+    <t>39.3417</t>
+  </si>
+  <si>
+    <t>43.52073</t>
+  </si>
+  <si>
+    <t>39.634758</t>
+  </si>
+  <si>
+    <t>42.952835</t>
+  </si>
+  <si>
+    <t>31.53167</t>
+  </si>
+  <si>
+    <t>29.056887</t>
+  </si>
+  <si>
+    <t>29.729128</t>
+  </si>
+  <si>
+    <t>37.555595</t>
+  </si>
+  <si>
+    <t>29.474957</t>
+  </si>
+  <si>
+    <t>31.044846</t>
+  </si>
+  <si>
+    <t>37.67582</t>
   </si>
 </sst>
 </file>
@@ -443,7 +1274,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7B237B-FD1A-6540-8185-F12A1750F307}">
-  <dimension ref="D107:G111"/>
+  <dimension ref="D107:G144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,58 +1296,520 @@
     </row>
     <row r="108">
       <c r="D108" t="s">
-        <v>1</v>
+        <v>167</v>
       </c>
       <c r="E108" t="s">
-        <v>6</v>
+        <v>204</v>
       </c>
       <c r="F108" t="s">
-        <v>11</v>
+        <v>239</v>
       </c>
       <c r="G108" t="s">
-        <v>16</v>
+        <v>276</v>
       </c>
     </row>
     <row r="109">
       <c r="D109" t="s">
-        <v>2</v>
+        <v>168</v>
       </c>
       <c r="E109" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
       <c r="F109" t="s">
-        <v>12</v>
+        <v>240</v>
       </c>
       <c r="G109" t="s">
-        <v>17</v>
+        <v>277</v>
       </c>
     </row>
     <row r="110">
       <c r="D110" t="s">
-        <v>3</v>
+        <v>169</v>
       </c>
       <c r="E110" t="s">
-        <v>8</v>
+        <v>206</v>
       </c>
       <c r="F110" t="s">
-        <v>13</v>
+        <v>241</v>
       </c>
       <c r="G110" t="s">
-        <v>18</v>
+        <v>278</v>
       </c>
     </row>
     <row r="111">
       <c r="D111" t="s">
-        <v>4</v>
+        <v>170</v>
       </c>
       <c r="E111" t="s">
-        <v>9</v>
+        <v>207</v>
       </c>
       <c r="F111" t="s">
-        <v>14</v>
+        <v>242</v>
       </c>
       <c r="G111" t="s">
-        <v>19</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="D112" t="s">
+        <v>171</v>
+      </c>
+      <c r="E112" t="s">
+        <v>208</v>
+      </c>
+      <c r="F112" t="s">
+        <v>243</v>
+      </c>
+      <c r="G112" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="D113" t="s">
+        <v>172</v>
+      </c>
+      <c r="E113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F113" t="s">
+        <v>244</v>
+      </c>
+      <c r="G113" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="D114" t="s">
+        <v>173</v>
+      </c>
+      <c r="E114" t="s">
+        <v>70</v>
+      </c>
+      <c r="F114" t="s">
+        <v>245</v>
+      </c>
+      <c r="G114" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="D115" t="s">
+        <v>174</v>
+      </c>
+      <c r="E115" t="s">
+        <v>209</v>
+      </c>
+      <c r="F115" t="s">
+        <v>246</v>
+      </c>
+      <c r="G115" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="D116" t="s">
+        <v>175</v>
+      </c>
+      <c r="E116" t="s">
+        <v>210</v>
+      </c>
+      <c r="F116" t="s">
+        <v>247</v>
+      </c>
+      <c r="G116" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="D117" t="s">
+        <v>176</v>
+      </c>
+      <c r="E117" t="s">
+        <v>211</v>
+      </c>
+      <c r="F117" t="s">
+        <v>248</v>
+      </c>
+      <c r="G117" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="D118" t="s">
+        <v>177</v>
+      </c>
+      <c r="E118" t="s">
+        <v>212</v>
+      </c>
+      <c r="F118" t="s">
+        <v>249</v>
+      </c>
+      <c r="G118" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="D119" t="s">
+        <v>178</v>
+      </c>
+      <c r="E119" t="s">
+        <v>213</v>
+      </c>
+      <c r="F119" t="s">
+        <v>250</v>
+      </c>
+      <c r="G119" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="D120" t="s">
+        <v>179</v>
+      </c>
+      <c r="E120" t="s">
+        <v>214</v>
+      </c>
+      <c r="F120" t="s">
+        <v>251</v>
+      </c>
+      <c r="G120" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="D121" t="s">
+        <v>180</v>
+      </c>
+      <c r="E121" t="s">
+        <v>215</v>
+      </c>
+      <c r="F121" t="s">
+        <v>252</v>
+      </c>
+      <c r="G121" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="D122" t="s">
+        <v>181</v>
+      </c>
+      <c r="E122" t="s">
+        <v>216</v>
+      </c>
+      <c r="F122" t="s">
+        <v>253</v>
+      </c>
+      <c r="G122" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="D123" t="s">
+        <v>182</v>
+      </c>
+      <c r="E123" t="s">
+        <v>217</v>
+      </c>
+      <c r="F123" t="s">
+        <v>254</v>
+      </c>
+      <c r="G123" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="D124" t="s">
+        <v>183</v>
+      </c>
+      <c r="E124" t="s">
+        <v>218</v>
+      </c>
+      <c r="F124" t="s">
+        <v>255</v>
+      </c>
+      <c r="G124" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="D125" t="s">
+        <v>184</v>
+      </c>
+      <c r="E125" t="s">
+        <v>219</v>
+      </c>
+      <c r="F125" t="s">
+        <v>256</v>
+      </c>
+      <c r="G125" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="D126" t="s">
+        <v>185</v>
+      </c>
+      <c r="E126" t="s">
+        <v>220</v>
+      </c>
+      <c r="F126" t="s">
+        <v>257</v>
+      </c>
+      <c r="G126" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="D127" t="s">
+        <v>186</v>
+      </c>
+      <c r="E127" t="s">
+        <v>221</v>
+      </c>
+      <c r="F127" t="s">
+        <v>258</v>
+      </c>
+      <c r="G127" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="D128" t="s">
+        <v>187</v>
+      </c>
+      <c r="E128" t="s">
+        <v>222</v>
+      </c>
+      <c r="F128" t="s">
+        <v>259</v>
+      </c>
+      <c r="G128" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="D129" t="s">
+        <v>152</v>
+      </c>
+      <c r="E129" t="s">
+        <v>188</v>
+      </c>
+      <c r="F129" t="s">
+        <v>223</v>
+      </c>
+      <c r="G129" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="D130" t="s">
+        <v>153</v>
+      </c>
+      <c r="E130" t="s">
+        <v>189</v>
+      </c>
+      <c r="F130" t="s">
+        <v>224</v>
+      </c>
+      <c r="G130" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="D131" t="s">
+        <v>154</v>
+      </c>
+      <c r="E131" t="s">
+        <v>190</v>
+      </c>
+      <c r="F131" t="s">
+        <v>225</v>
+      </c>
+      <c r="G131" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="D132" t="s">
+        <v>155</v>
+      </c>
+      <c r="E132" t="s">
+        <v>191</v>
+      </c>
+      <c r="F132" t="s">
+        <v>226</v>
+      </c>
+      <c r="G132" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="D133" t="s">
+        <v>156</v>
+      </c>
+      <c r="E133" t="s">
+        <v>192</v>
+      </c>
+      <c r="F133" t="s">
+        <v>227</v>
+      </c>
+      <c r="G133" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="D134" t="s">
+        <v>157</v>
+      </c>
+      <c r="E134" t="s">
+        <v>193</v>
+      </c>
+      <c r="F134" t="s">
+        <v>228</v>
+      </c>
+      <c r="G134" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="D135" t="s">
+        <v>158</v>
+      </c>
+      <c r="E135" t="s">
+        <v>194</v>
+      </c>
+      <c r="F135" t="s">
+        <v>229</v>
+      </c>
+      <c r="G135" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="D136" t="s">
+        <v>23</v>
+      </c>
+      <c r="E136" t="s">
+        <v>195</v>
+      </c>
+      <c r="F136" t="s">
+        <v>230</v>
+      </c>
+      <c r="G136" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="D137" t="s">
+        <v>159</v>
+      </c>
+      <c r="E137" t="s">
+        <v>196</v>
+      </c>
+      <c r="F137" t="s">
+        <v>231</v>
+      </c>
+      <c r="G137" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="D138" t="s">
+        <v>160</v>
+      </c>
+      <c r="E138" t="s">
+        <v>197</v>
+      </c>
+      <c r="F138" t="s">
+        <v>232</v>
+      </c>
+      <c r="G138" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="D139" t="s">
+        <v>161</v>
+      </c>
+      <c r="E139" t="s">
+        <v>198</v>
+      </c>
+      <c r="F139" t="s">
+        <v>233</v>
+      </c>
+      <c r="G139" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="D140" t="s">
+        <v>162</v>
+      </c>
+      <c r="E140" t="s">
+        <v>199</v>
+      </c>
+      <c r="F140" t="s">
+        <v>234</v>
+      </c>
+      <c r="G140" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="D141" t="s">
+        <v>163</v>
+      </c>
+      <c r="E141" t="s">
+        <v>200</v>
+      </c>
+      <c r="F141" t="s">
+        <v>235</v>
+      </c>
+      <c r="G141" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="D142" t="s">
+        <v>164</v>
+      </c>
+      <c r="E142" t="s">
+        <v>201</v>
+      </c>
+      <c r="F142" t="s">
+        <v>236</v>
+      </c>
+      <c r="G142" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="D143" t="s">
+        <v>165</v>
+      </c>
+      <c r="E143" t="s">
+        <v>202</v>
+      </c>
+      <c r="F143" t="s">
+        <v>237</v>
+      </c>
+      <c r="G143" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="D144" t="s">
+        <v>166</v>
+      </c>
+      <c r="E144" t="s">
+        <v>203</v>
+      </c>
+      <c r="F144" t="s">
+        <v>238</v>
+      </c>
+      <c r="G144" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>